<commit_message>
extensions of lag analysis complete
</commit_message>
<xml_diff>
--- a/Lags/Outputs/dtw_results/dtw_summary.xlsx
+++ b/Lags/Outputs/dtw_results/dtw_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliebloom/Desktop/Masters/Project/Analysis/Lags/Outputs/dtw_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A36E192-A8D4-4747-B103-A804C1C75C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C86A00F-3A2D-B94B-ACF1-232BEE19B9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30240" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{4AA3BF32-F25C-CF4F-B4C5-A1818573DF45}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="20">
   <si>
     <t>Lockdown 1</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Open DTW</t>
+  </si>
+  <si>
+    <t>Standard dates</t>
+  </si>
+  <si>
+    <t>Now need to try with the flexed dates - add maybe 3 days before and after to take into account premature drop and also the 7-day moving average. Or make it a week before to round off more?</t>
   </si>
 </sst>
 </file>
@@ -874,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B332B296-8431-C841-B1D5-CBB40E4B1809}">
-  <dimension ref="B2:J6"/>
+  <dimension ref="B2:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -886,138 +892,148 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="18" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="19"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="15" t="s">
+      <c r="J3" s="19"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J4" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="16">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="16">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C5" s="5">
         <f>Standard!D1</f>
         <v>0.31372549019607843</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D5" s="6">
         <f>Standard!D2</f>
         <v>0</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="5">
-        <f>Open!D1</f>
-        <v>-6.25E-2</v>
-      </c>
-      <c r="J4" s="7">
-        <f>Open!D2</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="16">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5">
-        <f>Standard!I1</f>
-        <v>2.4761904761904763</v>
-      </c>
-      <c r="D5" s="6">
-        <f>Standard!I2</f>
-        <v>2</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="7"/>
       <c r="I5" s="5">
+        <f>Open!D1</f>
+        <v>-6.25E-2</v>
+      </c>
+      <c r="J5" s="7">
+        <f>Open!D2</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="16">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5">
+        <f>Standard!I1</f>
+        <v>2.4761904761904763</v>
+      </c>
+      <c r="D6" s="6">
+        <f>Standard!I2</f>
+        <v>2</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="5">
         <f>Open!I1</f>
         <v>3.3571428571428572</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J6" s="7">
         <f>Open!I2</f>
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="17">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="17">
         <v>3</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C7" s="8">
         <f>Standard!N1</f>
         <v>-1.7248677248677249</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D7" s="9">
         <f>Standard!N2</f>
         <v>1</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E7" s="10">
         <f>Standard!R6</f>
         <v>14.246753246753247</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F7" s="10">
         <f>Standard!R7</f>
         <v>-12.705357142857142</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G7" s="10">
         <f>Standard!R8</f>
         <v>15</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H7" s="11">
         <f>Standard!R9</f>
         <v>-12.5</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I7" s="8">
         <f>Open!N1</f>
         <v>33.169811320754718</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J7" s="22">
         <f>Open!N2</f>
         <v>33.5</v>
       </c>
     </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>